<commit_message>
- Add choice to practise (verb forms or words) - unique selection
</commit_message>
<xml_diff>
--- a/Spanish.xlsx
+++ b/Spanish.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23211"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47850DED-785C-4BDB-B34A-713B7428DE8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E9CD8A4-CF35-481A-9EDD-16AD554FCAD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="620">
   <si>
     <t>yo</t>
   </si>
@@ -694,19 +694,19 @@
     <t>mostrar</t>
   </si>
   <si>
-    <t>muesto</t>
-  </si>
-  <si>
-    <t>mostás</t>
-  </si>
-  <si>
-    <t>muesta</t>
-  </si>
-  <si>
-    <t>mostamos</t>
-  </si>
-  <si>
-    <t>muestan</t>
+    <t>muestro</t>
+  </si>
+  <si>
+    <t>mostrás</t>
+  </si>
+  <si>
+    <t>muestra</t>
+  </si>
+  <si>
+    <t>mostramos</t>
+  </si>
+  <si>
+    <t>muestran</t>
   </si>
   <si>
     <t>to show</t>
@@ -1351,151 +1351,541 @@
     <t>to fly</t>
   </si>
   <si>
-    <t>cuaderno</t>
+    <t>el cuaderno</t>
   </si>
   <si>
     <t>notebook</t>
   </si>
   <si>
-    <t>regla</t>
+    <t>la regla</t>
   </si>
   <si>
     <t>ruler</t>
   </si>
   <si>
-    <t>cinta de papel</t>
+    <t>la cinta de papel</t>
   </si>
   <si>
     <t>paper tape</t>
   </si>
   <si>
-    <t>calculadora</t>
+    <t>la calculadora</t>
   </si>
   <si>
     <t>calculator</t>
   </si>
   <si>
-    <t>lápiz</t>
+    <t>el lápiz</t>
   </si>
   <si>
     <t>pencil</t>
   </si>
   <si>
-    <t>plasticola</t>
+    <t>la plasticola</t>
   </si>
   <si>
     <t>glue</t>
   </si>
   <si>
-    <t>pincel</t>
+    <t>el pincel</t>
   </si>
   <si>
     <t>paintbrush</t>
   </si>
   <si>
-    <t>lapicero</t>
+    <t>el lapicero</t>
   </si>
   <si>
     <t>pen holder</t>
   </si>
   <si>
-    <t>tijera</t>
+    <t>la tijera</t>
   </si>
   <si>
     <t>scissors</t>
   </si>
   <si>
-    <t>libro</t>
+    <t>el libro</t>
   </si>
   <si>
     <t>book</t>
   </si>
   <si>
-    <t>resaltador</t>
+    <t>el resaltador</t>
   </si>
   <si>
     <t>highlighter pen</t>
   </si>
   <si>
-    <t>perforadora</t>
+    <t>la perforadora</t>
   </si>
   <si>
     <t>puncher</t>
   </si>
   <si>
-    <t>goma</t>
+    <t>la goma</t>
   </si>
   <si>
     <t>eraser</t>
   </si>
   <si>
-    <t>hojas de papel</t>
+    <t>las hojas de papel</t>
   </si>
   <si>
     <t>paper sheets</t>
   </si>
   <si>
-    <t>sacapuntas</t>
+    <t>el sacapuntas</t>
   </si>
   <si>
     <t>sharpener</t>
   </si>
   <si>
-    <t>escritorio</t>
+    <t>el escritorio</t>
   </si>
   <si>
     <t>desk</t>
   </si>
   <si>
-    <t>tacho de basura</t>
+    <t>el tacho de basura</t>
   </si>
   <si>
     <t>trash can</t>
   </si>
   <si>
-    <t>reloj</t>
+    <t>el reloj</t>
   </si>
   <si>
     <t>clock</t>
   </si>
   <si>
-    <t>abrochadora</t>
+    <t>la abrochadora</t>
   </si>
   <si>
     <t>stapler</t>
   </si>
   <si>
-    <t>carpeta</t>
+    <t>la carpeta</t>
   </si>
   <si>
     <t>folder</t>
   </si>
   <si>
-    <t>computadora portátil</t>
+    <t>la computadora portátil</t>
   </si>
   <si>
     <t>laptop</t>
   </si>
   <si>
-    <t>agenda</t>
+    <t>la agenda</t>
   </si>
   <si>
     <t>schedule</t>
   </si>
   <si>
-    <t>lapicera</t>
+    <t>la lapicera</t>
   </si>
   <si>
     <t>pen</t>
   </si>
   <si>
-    <t>impresora</t>
+    <t>la impresora</t>
   </si>
   <si>
     <t>printer</t>
   </si>
   <si>
-    <t>bolígrafo</t>
+    <t>el bolígrafo</t>
+  </si>
+  <si>
+    <t>el dormitorio</t>
+  </si>
+  <si>
+    <t>bedroom</t>
+  </si>
+  <si>
+    <t>la cama</t>
+  </si>
+  <si>
+    <t>bed</t>
+  </si>
+  <si>
+    <t>la lámpara</t>
+  </si>
+  <si>
+    <t>lamp</t>
+  </si>
+  <si>
+    <t>la mesita de luz</t>
+  </si>
+  <si>
+    <t>nightstand</t>
+  </si>
+  <si>
+    <t>la cuadro</t>
+  </si>
+  <si>
+    <t>picture/painting[c]</t>
+  </si>
+  <si>
+    <t>la pintura</t>
+  </si>
+  <si>
+    <t>painting [p]</t>
+  </si>
+  <si>
+    <t>el espejo</t>
+  </si>
+  <si>
+    <t>mirror</t>
+  </si>
+  <si>
+    <t>el quarto de baño</t>
+  </si>
+  <si>
+    <t>bathroom</t>
+  </si>
+  <si>
+    <t>la bañera</t>
+  </si>
+  <si>
+    <t>bathtub</t>
+  </si>
+  <si>
+    <t>el inodoro</t>
+  </si>
+  <si>
+    <t>toilet</t>
+  </si>
+  <si>
+    <t>la alfombrilla</t>
+  </si>
+  <si>
+    <t>mat</t>
+  </si>
+  <si>
+    <t>el lavabo</t>
+  </si>
+  <si>
+    <t>sink (to wash hands)</t>
+  </si>
+  <si>
+    <t>la ducha</t>
+  </si>
+  <si>
+    <t>shower</t>
+  </si>
+  <si>
+    <t>la toalla</t>
+  </si>
+  <si>
+    <t>towel</t>
+  </si>
+  <si>
+    <t>el salón</t>
+  </si>
+  <si>
+    <t>living room [s]</t>
+  </si>
+  <si>
+    <t>la puerta</t>
+  </si>
+  <si>
+    <t>door</t>
+  </si>
+  <si>
+    <t>el sillón</t>
+  </si>
+  <si>
+    <t>arnchair</t>
+  </si>
+  <si>
+    <t>el sofa</t>
+  </si>
+  <si>
+    <t>sofa</t>
+  </si>
+  <si>
+    <t>el suelo</t>
+  </si>
+  <si>
+    <t>soil</t>
+  </si>
+  <si>
+    <t>el piso</t>
+  </si>
+  <si>
+    <t>floor</t>
+  </si>
+  <si>
+    <t>la silla</t>
+  </si>
+  <si>
+    <t>chair</t>
+  </si>
+  <si>
+    <t>la planta</t>
+  </si>
+  <si>
+    <t>plant</t>
+  </si>
+  <si>
+    <t>la mesa</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>el armario</t>
+  </si>
+  <si>
+    <t>cabinet</t>
+  </si>
+  <si>
+    <t>la estantería</t>
+  </si>
+  <si>
+    <t>shelf</t>
+  </si>
+  <si>
+    <t>el techo</t>
+  </si>
+  <si>
+    <t>ceiling/roof</t>
+  </si>
+  <si>
+    <t>la chimenea</t>
+  </si>
+  <si>
+    <t>chimney</t>
+  </si>
+  <si>
+    <t>la ventana</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>la cocina</t>
+  </si>
+  <si>
+    <t>kitchen</t>
+  </si>
+  <si>
+    <t>la heladera</t>
+  </si>
+  <si>
+    <t>refrigerator</t>
+  </si>
+  <si>
+    <t>el horno</t>
+  </si>
+  <si>
+    <t>oven</t>
+  </si>
+  <si>
+    <t>el lavarropas</t>
+  </si>
+  <si>
+    <t>washing machine</t>
+  </si>
+  <si>
+    <t>el microondas</t>
+  </si>
+  <si>
+    <t>microwave</t>
+  </si>
+  <si>
+    <t>el lavatorio</t>
+  </si>
+  <si>
+    <t>sink (for kitchen)</t>
+  </si>
+  <si>
+    <t>el lavavajillas</t>
+  </si>
+  <si>
+    <t>dishwasher</t>
+  </si>
+  <si>
+    <t>el cajón</t>
+  </si>
+  <si>
+    <t>drawer</t>
+  </si>
+  <si>
+    <t>el auto</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>el garaje</t>
+  </si>
+  <si>
+    <t>garage</t>
+  </si>
+  <si>
+    <t>el baño</t>
+  </si>
+  <si>
+    <t>bath</t>
+  </si>
+  <si>
+    <t>el living</t>
+  </si>
+  <si>
+    <t>living room [l]</t>
+  </si>
+  <si>
+    <t>en el centro de</t>
+  </si>
+  <si>
+    <t>in the center of</t>
+  </si>
+  <si>
+    <t>encima de</t>
+  </si>
+  <si>
+    <t>above of/on [e]</t>
+  </si>
+  <si>
+    <t>sobre</t>
+  </si>
+  <si>
+    <t>on [s]</t>
+  </si>
+  <si>
+    <t>abajo de</t>
+  </si>
+  <si>
+    <t>under of</t>
+  </si>
+  <si>
+    <t>a la derecha de</t>
+  </si>
+  <si>
+    <t>to the right of</t>
+  </si>
+  <si>
+    <t>a la izquierda de</t>
+  </si>
+  <si>
+    <t>to the left of</t>
+  </si>
+  <si>
+    <t>entre y</t>
+  </si>
+  <si>
+    <t>between and</t>
+  </si>
+  <si>
+    <t>al lado de</t>
+  </si>
+  <si>
+    <t>next to</t>
+  </si>
+  <si>
+    <t>adelante de</t>
+  </si>
+  <si>
+    <t>in front of</t>
+  </si>
+  <si>
+    <t>atrás de</t>
+  </si>
+  <si>
+    <t>behind of</t>
+  </si>
+  <si>
+    <t>alrededor de</t>
+  </si>
+  <si>
+    <t>around (the house)</t>
+  </si>
+  <si>
+    <t>la bicicleta</t>
+  </si>
+  <si>
+    <t>bicycle</t>
+  </si>
+  <si>
+    <t>la pelota</t>
+  </si>
+  <si>
+    <t>ball</t>
+  </si>
+  <si>
+    <t>las zapatos</t>
+  </si>
+  <si>
+    <t>shoes</t>
+  </si>
+  <si>
+    <t>el ratón</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>la serpiente</t>
+  </si>
+  <si>
+    <t>snake</t>
+  </si>
+  <si>
+    <t>el pájaro</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>la falda</t>
+  </si>
+  <si>
+    <t>skirt</t>
+  </si>
+  <si>
+    <t>la banda</t>
+  </si>
+  <si>
+    <t>(music) band</t>
+  </si>
+  <si>
+    <t>la maleta</t>
+  </si>
+  <si>
+    <t>suitcase</t>
+  </si>
+  <si>
+    <t>el periódico</t>
+  </si>
+  <si>
+    <t>newspaper</t>
+  </si>
+  <si>
+    <t>closet</t>
+  </si>
+  <si>
+    <t>el bocadillo</t>
+  </si>
+  <si>
+    <t>snack</t>
+  </si>
+  <si>
+    <t>la haladera</t>
+  </si>
+  <si>
+    <t>la libreta</t>
+  </si>
+  <si>
+    <t>notepad</t>
+  </si>
+  <si>
+    <t>la camisa</t>
+  </si>
+  <si>
+    <t>shirt</t>
   </si>
 </sst>
 </file>
@@ -1850,8 +2240,8 @@
   <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3372,15 +3762,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879A71AB-1072-4E7D-9CD5-E80124DBA1D6}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3584,6 +3974,534 @@
         <v>486</v>
       </c>
     </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>490</v>
+      </c>
+      <c r="B26" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>492</v>
+      </c>
+      <c r="B27" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>494</v>
+      </c>
+      <c r="B28" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>496</v>
+      </c>
+      <c r="B29" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>498</v>
+      </c>
+      <c r="B30" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>500</v>
+      </c>
+      <c r="B31" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>502</v>
+      </c>
+      <c r="B32" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>504</v>
+      </c>
+      <c r="B33" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>506</v>
+      </c>
+      <c r="B34" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>508</v>
+      </c>
+      <c r="B35" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>510</v>
+      </c>
+      <c r="B36" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>512</v>
+      </c>
+      <c r="B37" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>514</v>
+      </c>
+      <c r="B38" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>516</v>
+      </c>
+      <c r="B39" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>518</v>
+      </c>
+      <c r="B40" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>520</v>
+      </c>
+      <c r="B41" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>522</v>
+      </c>
+      <c r="B42" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>524</v>
+      </c>
+      <c r="B43" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>526</v>
+      </c>
+      <c r="B44" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>528</v>
+      </c>
+      <c r="B45" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>530</v>
+      </c>
+      <c r="B46" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>532</v>
+      </c>
+      <c r="B47" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>534</v>
+      </c>
+      <c r="B48" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>536</v>
+      </c>
+      <c r="B49" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>538</v>
+      </c>
+      <c r="B50" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>540</v>
+      </c>
+      <c r="B51" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>542</v>
+      </c>
+      <c r="B52" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>544</v>
+      </c>
+      <c r="B53" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>546</v>
+      </c>
+      <c r="B54" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>548</v>
+      </c>
+      <c r="B55" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>550</v>
+      </c>
+      <c r="B56" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>552</v>
+      </c>
+      <c r="B57" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>554</v>
+      </c>
+      <c r="B58" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>556</v>
+      </c>
+      <c r="B59" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>558</v>
+      </c>
+      <c r="B60" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>560</v>
+      </c>
+      <c r="B61" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>562</v>
+      </c>
+      <c r="B62" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>564</v>
+      </c>
+      <c r="B63" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>566</v>
+      </c>
+      <c r="B64" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>568</v>
+      </c>
+      <c r="B65" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>570</v>
+      </c>
+      <c r="B66" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>572</v>
+      </c>
+      <c r="B67" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>574</v>
+      </c>
+      <c r="B68" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>576</v>
+      </c>
+      <c r="B69" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>578</v>
+      </c>
+      <c r="B70" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>580</v>
+      </c>
+      <c r="B71" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>582</v>
+      </c>
+      <c r="B72" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>584</v>
+      </c>
+      <c r="B73" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>586</v>
+      </c>
+      <c r="B74" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>588</v>
+      </c>
+      <c r="B75" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>590</v>
+      </c>
+      <c r="B76" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>592</v>
+      </c>
+      <c r="B77" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>594</v>
+      </c>
+      <c r="B78" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>596</v>
+      </c>
+      <c r="B79" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>598</v>
+      </c>
+      <c r="B80" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>600</v>
+      </c>
+      <c r="B81" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>602</v>
+      </c>
+      <c r="B82" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>604</v>
+      </c>
+      <c r="B83" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>606</v>
+      </c>
+      <c r="B84" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>608</v>
+      </c>
+      <c r="B85" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>610</v>
+      </c>
+      <c r="B86" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>536</v>
+      </c>
+      <c r="B87" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>613</v>
+      </c>
+      <c r="B88" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>615</v>
+      </c>
+      <c r="B89" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>616</v>
+      </c>
+      <c r="B90" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>618</v>
+      </c>
+      <c r="B91" t="s">
+        <v>619</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Update words sheet - Add unique counter (not really good though.... still too much duplicate)
</commit_message>
<xml_diff>
--- a/Spanish.xlsx
+++ b/Spanish.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23211"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E9CD8A4-CF35-481A-9EDD-16AD554FCAD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAA942E9-1AD2-4DE5-AB6A-A2CD172D55CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verbs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="622">
   <si>
     <t>yo</t>
   </si>
@@ -1486,7 +1486,7 @@
     <t>la lapicera</t>
   </si>
   <si>
-    <t>pen</t>
+    <t>pen (l)</t>
   </si>
   <si>
     <t>la impresora</t>
@@ -1498,6 +1498,9 @@
     <t>el bolígrafo</t>
   </si>
   <si>
+    <t>pen (b)</t>
+  </si>
+  <si>
     <t>el dormitorio</t>
   </si>
   <si>
@@ -1522,7 +1525,7 @@
     <t>nightstand</t>
   </si>
   <si>
-    <t>la cuadro</t>
+    <t>el cuadro</t>
   </si>
   <si>
     <t>picture/painting[c]</t>
@@ -1816,7 +1819,7 @@
     <t>ball</t>
   </si>
   <si>
-    <t>las zapatos</t>
+    <t>los zapatos</t>
   </si>
   <si>
     <t>shoes</t>
@@ -1886,6 +1889,9 @@
   </si>
   <si>
     <t>shirt</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -2240,7 +2246,7 @@
   <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="D31" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
@@ -3762,10 +3768,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879A71AB-1072-4E7D-9CD5-E80124DBA1D6}">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3971,535 +3977,540 @@
         <v>489</v>
       </c>
       <c r="B25" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B26" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B27" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B28" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B29" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B30" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B31" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B32" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B33" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B34" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B35" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B36" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B37" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B38" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B39" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B40" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B41" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B42" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B43" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B44" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B45" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B46" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B47" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B48" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B49" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B50" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B51" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B52" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B53" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B54" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B55" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B56" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B57" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B58" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B59" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B60" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B61" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B62" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B63" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B64" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B65" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B66" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B67" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B68" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B69" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B70" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B71" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B72" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B73" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B74" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B75" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B76" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B77" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B78" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B79" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B80" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B81" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B82" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B83" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B84" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B85" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B86" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B87" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B88" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B89" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B90" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B91" t="s">
-        <v>619</v>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="B92" t="s">
+        <v>621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>